<commit_message>
add workhome to testing template
</commit_message>
<xml_diff>
--- a/comoOdeCpp/tests/testthat/data/Template_CoMoCOVID-19App_v15.xlsx
+++ b/comoOdeCpp/tests/testthat/data/Template_CoMoCOVID-19App_v15.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="387">
   <si>
     <t>Template v13.2</t>
   </si>
@@ -3633,10 +3633,10 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8733333333333" defaultRowHeight="15.75" outlineLevelCol="5"/>
@@ -3945,23 +3945,23 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="3" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="B15" s="4">
-        <v>43876</v>
+        <v>43905</v>
       </c>
       <c r="C15" s="4">
-        <v>43905</v>
+        <v>44093</v>
       </c>
       <c r="D15" s="3">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E15" s="1" t="str">
-        <f>VLOOKUP(A15,HIDDEN!$E$2:$F$17,2,0)</f>
+        <f>VLOOKUP(A15,[2]HIDDEN!$E$2:$F$14,2,0)</f>
         <v>%</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -3969,13 +3969,13 @@
         <v>171</v>
       </c>
       <c r="B16" s="4">
-        <v>43906</v>
+        <v>43876</v>
       </c>
       <c r="C16" s="4">
-        <v>44196</v>
+        <v>43905</v>
       </c>
       <c r="D16" s="3">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="E16" s="1" t="str">
         <f>VLOOKUP(A16,HIDDEN!$E$2:$F$17,2,0)</f>
@@ -3987,16 +3987,16 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="3" t="s">
-        <v>152</v>
+        <v>171</v>
       </c>
       <c r="B17" s="4">
-        <v>43845</v>
+        <v>43906</v>
       </c>
       <c r="C17" s="4">
-        <v>43921</v>
+        <v>44196</v>
       </c>
       <c r="D17" s="3">
-        <v>60</v>
+        <v>5</v>
       </c>
       <c r="E17" s="1" t="str">
         <f>VLOOKUP(A17,HIDDEN!$E$2:$F$17,2,0)</f>
@@ -4008,10 +4008,10 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B18" s="4">
-        <v>43876</v>
+        <v>43845</v>
       </c>
       <c r="C18" s="4">
         <v>43921</v>
@@ -4021,7 +4021,7 @@
       </c>
       <c r="E18" s="1" t="str">
         <f>VLOOKUP(A18,HIDDEN!$E$2:$F$17,2,0)</f>
-        <v>contacts</v>
+        <v>%</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>229</v>
@@ -4029,20 +4029,20 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="3" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="B19" s="4">
         <v>43876</v>
       </c>
       <c r="C19" s="4">
-        <v>43982</v>
+        <v>43921</v>
       </c>
       <c r="D19" s="3">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="E19" s="1" t="str">
         <f>VLOOKUP(A19,HIDDEN!$E$2:$F$17,2,0)</f>
-        <v>%</v>
+        <v>contacts</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>229</v>
@@ -4050,20 +4050,20 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="3" t="s">
-        <v>200</v>
+        <v>160</v>
       </c>
       <c r="B20" s="4">
-        <v>43891</v>
+        <v>43876</v>
       </c>
       <c r="C20" s="4">
-        <v>44095</v>
+        <v>43982</v>
       </c>
       <c r="D20" s="3">
-        <v>10000</v>
+        <v>50</v>
       </c>
       <c r="E20" s="1" t="str">
         <f>VLOOKUP(A20,HIDDEN!$E$2:$F$17,2,0)</f>
-        <v>tests</v>
+        <v>%</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>229</v>
@@ -4071,20 +4071,20 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="3" t="s">
-        <v>241</v>
+        <v>200</v>
       </c>
       <c r="B21" s="4">
-        <v>43900</v>
+        <v>43891</v>
       </c>
       <c r="C21" s="4">
         <v>44095</v>
       </c>
       <c r="D21" s="3">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="E21" s="1" t="str">
         <f>VLOOKUP(A21,HIDDEN!$E$2:$F$17,2,0)</f>
-        <v>years</v>
+        <v>tests</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>229</v>
@@ -4092,16 +4092,16 @@
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="3" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B22" s="4">
-        <v>43891</v>
+        <v>43900</v>
       </c>
       <c r="C22" s="4">
         <v>44095</v>
       </c>
       <c r="D22" s="3">
-        <v>75</v>
+        <v>0</v>
       </c>
       <c r="E22" s="1" t="str">
         <f>VLOOKUP(A22,HIDDEN!$E$2:$F$17,2,0)</f>
@@ -4113,7 +4113,7 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B23" s="4">
         <v>43891</v>
@@ -4122,7 +4122,7 @@
         <v>44095</v>
       </c>
       <c r="D23" s="3">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="E23" s="1" t="str">
         <f>VLOOKUP(A23,HIDDEN!$E$2:$F$17,2,0)</f>
@@ -4134,7 +4134,7 @@
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="3" t="s">
-        <v>193</v>
+        <v>245</v>
       </c>
       <c r="B24" s="4">
         <v>43891</v>
@@ -4143,11 +4143,11 @@
         <v>44095</v>
       </c>
       <c r="D24" s="3">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="E24" s="1" t="str">
         <f>VLOOKUP(A24,HIDDEN!$E$2:$F$17,2,0)</f>
-        <v>%</v>
+        <v>years</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>229</v>
@@ -4155,16 +4155,16 @@
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="3" t="s">
-        <v>247</v>
+        <v>193</v>
       </c>
       <c r="B25" s="4">
         <v>43891</v>
       </c>
       <c r="C25" s="4">
-        <v>44089</v>
+        <v>44095</v>
       </c>
       <c r="D25" s="3">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="E25" s="1" t="str">
         <f>VLOOKUP(A25,HIDDEN!$E$2:$F$17,2,0)</f>
@@ -4176,16 +4176,16 @@
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="3" t="s">
-        <v>209</v>
+        <v>247</v>
       </c>
       <c r="B26" s="4">
-        <v>43910</v>
+        <v>43891</v>
       </c>
       <c r="C26" s="4">
-        <v>44095</v>
+        <v>44089</v>
       </c>
       <c r="D26" s="3">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="E26" s="1" t="str">
         <f>VLOOKUP(A26,HIDDEN!$E$2:$F$17,2,0)</f>
@@ -4197,38 +4197,66 @@
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="B27" s="4">
+        <v>43910</v>
+      </c>
+      <c r="C27" s="4">
+        <v>44095</v>
+      </c>
+      <c r="D27" s="3">
+        <v>0</v>
+      </c>
+      <c r="E27" s="1" t="str">
+        <f>VLOOKUP(A27,HIDDEN!$E$2:$F$17,2,0)</f>
+        <v>%</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="B27" s="5">
+      <c r="B28" s="5">
         <v>43891</v>
       </c>
-      <c r="C27" s="5">
+      <c r="C28" s="5">
         <v>44089</v>
       </c>
-      <c r="D27" s="6">
+      <c r="D28" s="6">
         <v>20</v>
       </c>
-      <c r="E27" s="1" t="str">
-        <f>VLOOKUP(A27,[2]HIDDEN!$E$2:$F$14,2,0)</f>
+      <c r="E28" s="1" t="str">
+        <f>VLOOKUP(A28,[2]HIDDEN!$E$2:$F$14,2,0)</f>
         <v>%</v>
       </c>
-      <c r="F27" s="6" t="s">
+      <c r="F28" s="6" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="3"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="3"/>
-      <c r="F28" s="3"/>
-    </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="3"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="3"/>
-      <c r="F29" s="3"/>
+      <c r="A29" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="B29" s="4">
+        <v>43905</v>
+      </c>
+      <c r="C29" s="4">
+        <v>44093</v>
+      </c>
+      <c r="D29" s="3">
+        <v>50</v>
+      </c>
+      <c r="E29" s="1" t="str">
+        <f>VLOOKUP(A29,[2]HIDDEN!$E$2:$F$14,2,0)</f>
+        <v>%</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>229</v>
+      </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="3"/>
@@ -4272,31 +4300,38 @@
       <c r="D35" s="3"/>
       <c r="F35" s="3"/>
     </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="3"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="3"/>
+      <c r="F36" s="3"/>
+    </row>
   </sheetData>
   <dataValidations count="8">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A6 A15:A19">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A6 A16:A20">
       <formula1>HIDDEN!$E$2:$E$16</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A30:A35">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A31:A36">
       <formula1>HIDDEN!$E$2:$E$11</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F27">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F28 F29">
       <formula1>[1]HIDDEN!#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7:A13 A20:A26 A28:A29">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A30 A7:A13 A21:A27">
       <formula1>HIDDEN!$E$2:$E$17</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F14 F2:F13 F15:F26 F28:F35">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F14 F15 F2:F13 F16:F27 F30:F36">
       <formula1>HIDDEN!$G$2:$G$3</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="between" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D14 D27 D2:D6 D8:D13 D15:D19 D21:D26 D28:D35">
+    <dataValidation type="decimal" operator="between" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D14 D15 D28 D29 D2:D6 D8:D13 D16:D20 D22:D27 D30:D36">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A14 A27">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A14 A15 A28 A29">
       <formula1>[2]HIDDEN!#REF!</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="between" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7 D20">
+    <dataValidation type="decimal" operator="between" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7 D21">
       <formula1>0</formula1>
       <formula2>10000000</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
add school closure and social distancing to testing
</commit_message>
<xml_diff>
--- a/comoOdeCpp/tests/testthat/data/Template_CoMoCOVID-19App_v15.xlsx
+++ b/comoOdeCpp/tests/testthat/data/Template_CoMoCOVID-19App_v15.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="387">
   <si>
     <t>Template v13.2</t>
   </si>
@@ -2726,7 +2726,7 @@
   <sheetPr/>
   <dimension ref="A1:G153"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" topLeftCell="A63" workbookViewId="0">
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
@@ -3635,8 +3635,8 @@
   </sheetPr>
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A30" sqref="$A30:$XFD31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8733333333333" defaultRowHeight="15.75" outlineLevelCol="5"/>
@@ -4259,18 +4259,44 @@
       </c>
     </row>
     <row r="30" spans="1:6">
-      <c r="A30" s="3"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="3"/>
-      <c r="F30" s="3"/>
+      <c r="A30" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B30" s="4">
+        <v>43905</v>
+      </c>
+      <c r="C30" s="4">
+        <v>44196</v>
+      </c>
+      <c r="D30" s="3">
+        <v>25</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>229</v>
+      </c>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" s="3"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="3"/>
-      <c r="F31" s="3"/>
+      <c r="A31" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B31" s="4">
+        <v>43910</v>
+      </c>
+      <c r="C31" s="4">
+        <v>44094</v>
+      </c>
+      <c r="D31" s="3">
+        <v>85</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>229</v>
+      </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="3"/>
@@ -4312,23 +4338,23 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A6 A16:A20">
       <formula1>HIDDEN!$E$2:$E$16</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A31:A36">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A32:A36">
       <formula1>HIDDEN!$E$2:$E$11</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F28 F29">
       <formula1>[1]HIDDEN!#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A30 A7:A13 A21:A27">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7:A13 A21:A27">
       <formula1>HIDDEN!$E$2:$E$17</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F14 F15 F2:F13 F16:F27 F30:F36">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F14 F15 F2:F13 F16:F27 F32:F36">
       <formula1>HIDDEN!$G$2:$G$3</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="between" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D14 D15 D28 D29 D2:D6 D8:D13 D16:D20 D22:D27 D30:D36">
+    <dataValidation type="decimal" operator="between" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D14 D15 D28 D29 D30 D31 D2:D6 D8:D13 D16:D20 D22:D27 D32:D36">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A14 A15 A28 A29">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A14 A15 A28 A29 A30 F30 A31 F31">
       <formula1>[2]HIDDEN!#REF!</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="between" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7 D21">
@@ -7057,7 +7083,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelCol="4"/>
@@ -7423,7 +7449,7 @@
   </sheetPr>
   <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fix missing mort_col%ICUCV in dCMdt, add testing for mortality calculation
</commit_message>
<xml_diff>
--- a/comoOdeCpp/tests/testthat/data/Template_CoMoCOVID-19App_v15.xlsx
+++ b/comoOdeCpp/tests/testthat/data/Template_CoMoCOVID-19App_v15.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23400" windowHeight="12000" tabRatio="648" firstSheet="5" activeTab="10"/>
+    <workbookView windowWidth="23400" windowHeight="12000" tabRatio="704" firstSheet="5" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -1320,9 +1320,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
     <numFmt numFmtId="176" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="177" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="26">
@@ -1362,6 +1362,29 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -1371,67 +1394,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1460,9 +1423,69 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1477,37 +1500,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1560,7 +1560,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1572,7 +1572,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1584,13 +1590,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1602,79 +1632,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1692,7 +1650,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1710,25 +1674,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1740,7 +1734,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1834,11 +1834,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1847,7 +1853,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1868,6 +1874,30 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -1878,21 +1908,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1916,164 +1931,149 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="35" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -3635,8 +3635,8 @@
   </sheetPr>
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A30" sqref="$A30:$XFD31"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8733333333333" defaultRowHeight="15.75" outlineLevelCol="5"/>
@@ -7449,8 +7449,8 @@
   </sheetPr>
   <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelCol="5"/>

</xml_diff>